<commit_message>
feat: tabela montada e preenchida test off
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -650,8 +650,8 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="1" sqref="D5 E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>